<commit_message>
Removed redundant test files
</commit_message>
<xml_diff>
--- a/test-files/gene-name-modifications/mismatched-case-related-input.xlsx
+++ b/test-files/gene-name-modifications/mismatched-case-related-input.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="25480" windowHeight="13940" tabRatio="773" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="25480" windowHeight="13940" tabRatio="773" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2317,7 +2317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
@@ -4355,8 +4355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4505,7 +4505,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>

</xml_diff>